<commit_message>
Análise atualizada dos indicadores do não circulante
</commit_message>
<xml_diff>
--- a/Indicadores_Financeiros_Embraer.xlsx
+++ b/Indicadores_Financeiros_Embraer.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,221 +454,287 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Liquidez Corrente</t>
+          <t>Endividamento Total</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.521024850020576</v>
+        <v>2.61068036787363</v>
       </c>
       <c r="C2" t="n">
-        <v>2.077064802136016</v>
+        <v>2.65978964066897</v>
       </c>
       <c r="D2" t="n">
-        <v>1.789310541698855</v>
+        <v>2.590901228701166</v>
       </c>
       <c r="E2" t="n">
-        <v>1.651977222909604</v>
+        <v>2.547669704768785</v>
       </c>
       <c r="F2" t="n">
-        <v>1.474636428340116</v>
+        <v>2.535321483732147</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Liquidez Seca</t>
+          <t>Dependência Financeira (%)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.514304675282405</v>
+        <v>72.30438869921596</v>
       </c>
       <c r="C3" t="n">
-        <v>1.375041165775489</v>
+        <v>72.67602517675823</v>
       </c>
       <c r="D3" t="n">
-        <v>1.065399162577329</v>
+        <v>72.15183776130478</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9328475809047825</v>
+        <v>71.81248303200837</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8098056475339028</v>
+        <v>71.71402927282512</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Endividamento Geral (%)</t>
+          <t>Independência Financeira (%)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>72.30438869921596</v>
+        <v>27.69561130078404</v>
       </c>
       <c r="C4" t="n">
-        <v>72.67602517675823</v>
+        <v>27.32397482324178</v>
       </c>
       <c r="D4" t="n">
-        <v>72.15183776130478</v>
+        <v>27.84816223869519</v>
       </c>
       <c r="E4" t="n">
-        <v>71.81248303200837</v>
+        <v>28.18751696799164</v>
       </c>
       <c r="F4" t="n">
-        <v>71.71402927282512</v>
+        <v>28.28597072717488</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Composição Endividamento (%)</t>
+          <t>Capital Terceiros LP</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>31.92047674097177</v>
+        <v>1.777338748265412</v>
       </c>
       <c r="C5" t="n">
-        <v>38.3307744728862</v>
+        <v>1.640271672050957</v>
       </c>
       <c r="D5" t="n">
-        <v>43.96559761962482</v>
+        <v>1.451796019768496</v>
       </c>
       <c r="E5" t="n">
-        <v>47.33928547706061</v>
+        <v>1.341621070215703</v>
       </c>
       <c r="F5" t="n">
-        <v>52.08081462901178</v>
+        <v>1.214905401540097</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Margem Bruta (%)</t>
+          <t>Imobilização Capital Permanente</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12.25423541388645</v>
+        <v>0.5436158758912167</v>
       </c>
       <c r="C6" t="n">
-        <v>15.61160147430238</v>
+        <v>0.5841007837308343</v>
       </c>
       <c r="D6" t="n">
-        <v>20.0862467376222</v>
+        <v>0.6332860718162319</v>
       </c>
       <c r="E6" t="n">
-        <v>17.24743328521607</v>
+        <v>0.6642000495078371</v>
       </c>
       <c r="F6" t="n">
-        <v>18.01660639991211</v>
+        <v>0.7170454445870662</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Margem Operacional (%)</t>
+          <t>Imobilização PL</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-8.558666115731766</v>
+        <v>0.6924936979743261</v>
       </c>
       <c r="C7" t="n">
-        <v>4.652544000903408</v>
+        <v>0.6298966221302366</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.369369379742759</v>
+        <v>0.6069636238741689</v>
       </c>
       <c r="E7" t="n">
-        <v>5.831401193626308</v>
+        <v>0.6115588787180845</v>
       </c>
       <c r="F7" t="n">
-        <v>10.64843742016398</v>
+        <v>0.6117320399472587</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Margem Líquida (%)</t>
+          <t>Imobilização Recursos Não Correntes</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-18.30911419157669</v>
+        <v>0.506399173702311</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.180509406717026</v>
+        <v>0.5413007481956502</v>
       </c>
       <c r="D8" t="n">
-        <v>-4.465961137152987</v>
+        <v>0.5737451953735432</v>
       </c>
       <c r="E8" t="n">
-        <v>3.003981116115012</v>
+        <v>0.592655594514736</v>
       </c>
       <c r="F8" t="n">
-        <v>5.430842226554105</v>
+        <v>0.619949725220023</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>ROA (%)</t>
+          <t>Giro do Imobilizado</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-2.803384448797868</v>
+        <v>1.707850277633619</v>
       </c>
       <c r="C9" t="n">
-        <v>1.773398941590173</v>
+        <v>2.214638267166006</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.008247929558513</v>
+        <v>2.517534106021249</v>
       </c>
       <c r="E9" t="n">
-        <v>2.927808167028303</v>
+        <v>2.912558117819684</v>
       </c>
       <c r="F9" t="n">
-        <v>5.151783021070909</v>
+        <v>2.796014152384233</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>ROE (%)</t>
+          <t>Nível Automação (Imobilizado/Receita)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-21.65374177608858</v>
+        <v>0.5855314210479801</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.646802552087117</v>
+        <v>0.4515410100267366</v>
       </c>
       <c r="D10" t="n">
-        <v>-6.824219169318738</v>
+        <v>0.3972140824659633</v>
       </c>
       <c r="E10" t="n">
-        <v>5.350693497321513</v>
+        <v>0.343340788251323</v>
       </c>
       <c r="F10" t="n">
-        <v>9.288974679429796</v>
+        <v>0.3576519808196515</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Giro do Ativo</t>
+          <t>Liquidez Geral</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3275492244807798</v>
+        <v>0.8443156610764809</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3811675808430448</v>
+        <v>0.8386409868815722</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4255342954030992</v>
+        <v>0.8430252061048135</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5020762711761939</v>
+        <v>0.8477923465624001</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4838064795606014</v>
+        <v>0.8528273445922694</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Composição Endividamento LP (%)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>68.07952325902824</v>
+      </c>
+      <c r="C12" t="n">
+        <v>61.6692255271138</v>
+      </c>
+      <c r="D12" t="n">
+        <v>56.03440238037519</v>
+      </c>
+      <c r="E12" t="n">
+        <v>52.6607145229394</v>
+      </c>
+      <c r="F12" t="n">
+        <v>47.91918537098822</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Participação ANC no Ativo (%)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>41.81498450315775</v>
+      </c>
+      <c r="C13" t="n">
+        <v>42.13861736122597</v>
+      </c>
+      <c r="D13" t="n">
+        <v>43.2395148561486</v>
+      </c>
+      <c r="E13" t="n">
+        <v>43.84018130761216</v>
+      </c>
+      <c r="F13" t="n">
+        <v>44.92343442240518</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Alavancagem Financeira (PNC/PL)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1.777338748265412</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1.640271672050957</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.451796019768496</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.341621070215703</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.214905401540097</v>
       </c>
     </row>
   </sheetData>
@@ -682,7 +748,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -732,243 +798,331 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Estoque</t>
+          <t>AtivoNaoCirculante</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16192719.42654592</v>
+        <v>29141300.63507662</v>
       </c>
       <c r="C3" t="n">
-        <v>12832737.55185522</v>
+        <v>27650888.97605425</v>
       </c>
       <c r="D3" t="n">
-        <v>13300908.3863406</v>
+        <v>25044728.79473388</v>
       </c>
       <c r="E3" t="n">
-        <v>13351321.926</v>
+        <v>23942405.2206</v>
       </c>
       <c r="F3" t="n">
-        <v>18181138</v>
+        <v>32892812</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>AtivoTotal</t>
+          <t>AtivoImobilizado</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>69691047.31552862</v>
+        <v>13366071.25367216</v>
       </c>
       <c r="C4" t="n">
-        <v>65618880.5129077</v>
+        <v>11293848.89331861</v>
       </c>
       <c r="D4" t="n">
-        <v>57920929.21961301</v>
+        <v>9790271.260123599</v>
       </c>
       <c r="E4" t="n">
-        <v>54612924.7336</v>
+        <v>9414354.1516</v>
       </c>
       <c r="F4" t="n">
-        <v>73219718</v>
+        <v>12669526</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>PassivoCirculante</t>
+          <t>AtivoRealizavelLP</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>16084627.91634959</v>
+        <v>1995054.146192828</v>
       </c>
       <c r="C5" t="n">
-        <v>18279637.44694333</v>
+        <v>2026121.285431994</v>
       </c>
       <c r="D5" t="n">
-        <v>18373669.44346336</v>
+        <v>2354678.50797864</v>
       </c>
       <c r="E5" t="n">
-        <v>18565945.7574</v>
+        <v>2578961.465</v>
       </c>
       <c r="F5" t="n">
-        <v>27347016</v>
+        <v>4454043</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>PassivoNaoCirculante</t>
+          <t>AtivoTotal</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>34305057.82322473</v>
+        <v>69691047.31552862</v>
       </c>
       <c r="C6" t="n">
-        <v>29409556.67532437</v>
+        <v>65618880.5129077</v>
       </c>
       <c r="D6" t="n">
-        <v>23417345.436912</v>
+        <v>57920929.21961301</v>
       </c>
       <c r="E6" t="n">
-        <v>20652951.5502</v>
+        <v>54612924.7336</v>
       </c>
       <c r="F6" t="n">
-        <v>25161794</v>
+        <v>73219718</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>PatrimonioLiquido</t>
+          <t>PassivoCirculante</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>19301361.5759543</v>
+        <v>16084627.91634959</v>
       </c>
       <c r="C7" t="n">
-        <v>17929686.39064</v>
+        <v>18279637.44694333</v>
       </c>
       <c r="D7" t="n">
-        <v>16129914.33923764</v>
+        <v>18373669.44346336</v>
       </c>
       <c r="E7" t="n">
-        <v>15394027.426</v>
+        <v>18565945.7574</v>
       </c>
       <c r="F7" t="n">
-        <v>20710908</v>
+        <v>27347016</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>ReceitaLiquida</t>
+          <t>PassivoNaoCirculante</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>22827248.50145473</v>
+        <v>34305057.82322473</v>
       </c>
       <c r="C8" t="n">
-        <v>25011789.94273384</v>
+        <v>29409556.67532437</v>
       </c>
       <c r="D8" t="n">
-        <v>24647341.8045608</v>
+        <v>23417345.436912</v>
       </c>
       <c r="E8" t="n">
-        <v>27419853.60827202</v>
+        <v>20652951.5502</v>
       </c>
       <c r="F8" t="n">
-        <v>35424174</v>
+        <v>25161794</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>LucroBruto</t>
+          <t>PatrimonioLiquido</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2797304.76988113</v>
+        <v>19301361.5759543</v>
       </c>
       <c r="C9" t="n">
-        <v>3904740.967449251</v>
+        <v>17929686.39064</v>
       </c>
       <c r="D9" t="n">
-        <v>4950725.889129187</v>
+        <v>16129914.33923764</v>
       </c>
       <c r="E9" t="n">
-        <v>4729220.957990627</v>
+        <v>15394027.426</v>
       </c>
       <c r="F9" t="n">
-        <v>6382234</v>
+        <v>20710908</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>LucroOperacional</t>
+          <t>ReceitaLiquida</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1953707.982647893</v>
+        <v>22827248.50145473</v>
       </c>
       <c r="C10" t="n">
-        <v>1163684.532499225</v>
+        <v>25011789.94273384</v>
       </c>
       <c r="D10" t="n">
-        <v>-583986.5696378001</v>
+        <v>24647341.8045608</v>
       </c>
       <c r="E10" t="n">
-        <v>1598961.670603361</v>
+        <v>27419853.60827202</v>
       </c>
       <c r="F10" t="n">
-        <v>3772121</v>
+        <v>35424174</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>LucroLiquido</t>
+          <t>DepreciacaoAmortizacao</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-4179466.994926325</v>
+        <v>-4751012.752529023</v>
       </c>
       <c r="C11" t="n">
-        <v>-295266.5330622761</v>
+        <v>-2741056.434950025</v>
       </c>
       <c r="D11" t="n">
-        <v>-1100740.706332947</v>
+        <v>-5534712.458766987</v>
       </c>
       <c r="E11" t="n">
-        <v>823687.2244588722</v>
+        <v>-3130259.287387266</v>
       </c>
       <c r="F11" t="n">
-        <v>1923831</v>
+        <v>-2610113</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>LucroLiquidoSocios</t>
+          <t>LucroBruto</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-4202456.060603281</v>
+        <v>2797304.76988113</v>
       </c>
       <c r="C12" t="n">
-        <v>-303211.4930596658</v>
+        <v>3904740.967449251</v>
       </c>
       <c r="D12" t="n">
-        <v>-1002401.5926451</v>
+        <v>4950725.889129187</v>
       </c>
       <c r="E12" t="n">
-        <v>822851.3082848575</v>
+        <v>4729220.957990627</v>
       </c>
       <c r="F12" t="n">
-        <v>1918850</v>
+        <v>6382234</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
+          <t>LucroOperacional</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-1953707.982647893</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1163684.532499225</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-583986.5696378001</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1598961.670603361</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3772121</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>LucroLiquido</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>-4179466.994926325</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-295266.5330622761</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-1100740.706332947</v>
+      </c>
+      <c r="E14" t="n">
+        <v>823687.2244588722</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1923831</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
           <t>PassivoTotal</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B15" t="n">
         <v>50389685.73957432</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C15" t="n">
         <v>47689194.1222677</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D15" t="n">
         <v>41791014.88037536</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E15" t="n">
         <v>39218897.3076</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F15" t="n">
         <v>52508810</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>CapitalPermanente</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>53606419.39917903</v>
+      </c>
+      <c r="C16" t="n">
+        <v>47339243.06596437</v>
+      </c>
+      <c r="D16" t="n">
+        <v>39547259.77614964</v>
+      </c>
+      <c r="E16" t="n">
+        <v>36046978.9762</v>
+      </c>
+      <c r="F16" t="n">
+        <v>45872702</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>AtivoPermanente</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>13366071.25367216</v>
+      </c>
+      <c r="C17" t="n">
+        <v>11293848.89331861</v>
+      </c>
+      <c r="D17" t="n">
+        <v>9790271.260123599</v>
+      </c>
+      <c r="E17" t="n">
+        <v>9414354.1516</v>
+      </c>
+      <c r="F17" t="n">
+        <v>12669526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Análise de curto prazo e efeito tesoura
</commit_message>
<xml_diff>
--- a/Indicadores_Financeiros_Embraer.xlsx
+++ b/Indicadores_Financeiros_Embraer.xlsx
@@ -748,7 +748,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -974,154 +974,132 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>DepreciacaoAmortizacao</t>
+          <t>LucroBruto</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-4751012.752529023</v>
+        <v>2797304.76988113</v>
       </c>
       <c r="C11" t="n">
-        <v>-2741056.434950025</v>
+        <v>3904740.967449251</v>
       </c>
       <c r="D11" t="n">
-        <v>-5534712.458766987</v>
+        <v>4950725.889129187</v>
       </c>
       <c r="E11" t="n">
-        <v>-3130259.287387266</v>
+        <v>4729220.957990627</v>
       </c>
       <c r="F11" t="n">
-        <v>-2610113</v>
+        <v>6382234</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>LucroBruto</t>
+          <t>LucroOperacional</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2797304.76988113</v>
+        <v>-1953707.982647893</v>
       </c>
       <c r="C12" t="n">
-        <v>3904740.967449251</v>
+        <v>1163684.532499225</v>
       </c>
       <c r="D12" t="n">
-        <v>4950725.889129187</v>
+        <v>-583986.5696378001</v>
       </c>
       <c r="E12" t="n">
-        <v>4729220.957990627</v>
+        <v>1598961.670603361</v>
       </c>
       <c r="F12" t="n">
-        <v>6382234</v>
+        <v>3772121</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>LucroOperacional</t>
+          <t>LucroLiquido</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1953707.982647893</v>
+        <v>-4179466.994926325</v>
       </c>
       <c r="C13" t="n">
-        <v>1163684.532499225</v>
+        <v>-295266.5330622761</v>
       </c>
       <c r="D13" t="n">
-        <v>-583986.5696378001</v>
+        <v>-1100740.706332947</v>
       </c>
       <c r="E13" t="n">
-        <v>1598961.670603361</v>
+        <v>823687.2244588722</v>
       </c>
       <c r="F13" t="n">
-        <v>3772121</v>
+        <v>1923831</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>LucroLiquido</t>
+          <t>PassivoTotal</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-4179466.994926325</v>
+        <v>50389685.73957432</v>
       </c>
       <c r="C14" t="n">
-        <v>-295266.5330622761</v>
+        <v>47689194.1222677</v>
       </c>
       <c r="D14" t="n">
-        <v>-1100740.706332947</v>
+        <v>41791014.88037536</v>
       </c>
       <c r="E14" t="n">
-        <v>823687.2244588722</v>
+        <v>39218897.3076</v>
       </c>
       <c r="F14" t="n">
-        <v>1923831</v>
+        <v>52508810</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>PassivoTotal</t>
+          <t>CapitalPermanente</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>50389685.73957432</v>
+        <v>53606419.39917903</v>
       </c>
       <c r="C15" t="n">
-        <v>47689194.1222677</v>
+        <v>47339243.06596437</v>
       </c>
       <c r="D15" t="n">
-        <v>41791014.88037536</v>
+        <v>39547259.77614964</v>
       </c>
       <c r="E15" t="n">
-        <v>39218897.3076</v>
+        <v>36046978.9762</v>
       </c>
       <c r="F15" t="n">
-        <v>52508810</v>
+        <v>45872702</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>CapitalPermanente</t>
+          <t>AtivoPermanente</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>53606419.39917903</v>
+        <v>13366071.25367216</v>
       </c>
       <c r="C16" t="n">
-        <v>47339243.06596437</v>
+        <v>11293848.89331861</v>
       </c>
       <c r="D16" t="n">
-        <v>39547259.77614964</v>
+        <v>9790271.260123599</v>
       </c>
       <c r="E16" t="n">
-        <v>36046978.9762</v>
+        <v>9414354.1516</v>
       </c>
       <c r="F16" t="n">
-        <v>45872702</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>AtivoPermanente</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>13366071.25367216</v>
-      </c>
-      <c r="C17" t="n">
-        <v>11293848.89331861</v>
-      </c>
-      <c r="D17" t="n">
-        <v>9790271.260123599</v>
-      </c>
-      <c r="E17" t="n">
-        <v>9414354.1516</v>
-      </c>
-      <c r="F17" t="n">
         <v>12669526</v>
       </c>
     </row>

</xml_diff>